<commit_message>
más espacio para la revisón de documentos
</commit_message>
<xml_diff>
--- a/propuestas_resolucion.xlsx
+++ b/propuestas_resolucion.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="213">
   <si>
     <t>Nombre completo</t>
   </si>
@@ -678,52 +678,58 @@
     <t>La solicitud de beca se rechaza porque el PPE es menor al requisito mínimo de 0.5.</t>
   </si>
   <si>
-    <t>La solicitud de beca se aprueba con una deuda vencida de 581385.0.</t>
-  </si>
-  <si>
-    <t>La solicitud de beca se aprueba con base en la validación de documentos y existencia de deuda vencida.</t>
+    <t>La solicitud de beca se aprueba porque los documentos han sido validados por la Trabajadora Social y el estudiante tiene una deuda vencida mayor que 0.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se aprueba debido a que el estudiante tiene deuda vencida y los documentos han sido validados por la Trabajadora Social.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se aprueba porque los documentos han sido validados y el estudiante tiene una deuda vencida mayor que 0.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se rechaza porque el estudiante no cumple con el requisito mínimo de PPE.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se rechaza porque no hay deuda a cubrir en el sistema.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se rechaza porque no hay deuda a cubrir.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se aprueba debido a que el estudiante cumple con los requisitos necesarios y tiene una deuda vencida.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se aprueba tras la validación de documentos por la Trabajadora Social y la existencia de deuda vencida.</t>
   </si>
   <si>
     <t>La solicitud de beca se aprueba debido a que los documentos han sido validados por una Trabajadora Social y el estudiante tiene una deuda vencida mayor que 0.</t>
   </si>
   <si>
-    <t>La solicitud de beca se rechaza porque el estudiante no cumple con el requisito mínimo de PPE.</t>
-  </si>
-  <si>
-    <t>La solicitud de beca se rechaza porque no hay deuda a cubrir.</t>
-  </si>
-  <si>
-    <t>La solicitud de beca se aprueba porque los documentos han sido validados por una Trabajadora Social y el estudiante tiene una deuda vencida mayor que 0.</t>
-  </si>
-  <si>
-    <t>La solicitud de beca se aprueba debido a que el estudiante cumple con el requisito de PPE y tiene deuda vencida validada.</t>
-  </si>
-  <si>
     <t>La solicitud de beca se rechaza porque el estudiante no tiene deuda a cubrir.</t>
   </si>
   <si>
     <t>La solicitud de beca se rechaza porque el estudiante no tiene deuda vencida en el sistema.</t>
   </si>
   <si>
-    <t>La solicitud de beca se rechaza porque se sugiere rechazar la solicitud de la Trabajadora Social.</t>
+    <t>La solicitud de beca se rechaza porque el estudiante no tiene deuda vencida a cubrir.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se rechaza porque el PPE es menor a 0.5.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se rechaza porque, a pesar de que el PPE es mayor a 0.5, la Trabajadora Social sugiere rechazar la solicitud debido a la situación económica familiar.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se aprueba debido a que el estudiante cumple con los requisitos establecidos y presenta una deuda vencida superior a 0.</t>
   </si>
   <si>
     <t>La solicitud de beca se rechaza porque la deuda vencida en el sistema es 0.</t>
   </si>
   <si>
-    <t>La solicitud de beca se rechaza porque el PPE es menor al requisito mínimo.</t>
-  </si>
-  <si>
-    <t>La solicitud de beca se aprueba con base en la validación de documentos y la deuda vencida.</t>
-  </si>
-  <si>
-    <t>La solicitud de beca se rechaza porque el PPE del estudiante es menor a 0.5.</t>
-  </si>
-  <si>
-    <t>La solicitud de beca se rechaza porque el PPE es menor a 0.5.</t>
-  </si>
-  <si>
-    <t>La solicitud de beca se rechaza debido a que la información proporcionada es insuficiente para realizar una evaluación adecuada.</t>
+    <t>La solicitud de beca se rechaza porque no hay deuda vencida que cubrir.</t>
+  </si>
+  <si>
+    <t>La solicitud de beca se rechaza porque no hay suficiente información para procesar la solicitud.</t>
   </si>
   <si>
     <t>N/A</t>
@@ -735,79 +741,73 @@
     <t>El estudiante no cumple con el requisito mínimo de PPE.</t>
   </si>
   <si>
-    <t>El estudiante solicita una beca para cubrir su deuda vencida y ha sido ayudado por la Trabajadora Social quien considera su situación económica.</t>
-  </si>
-  <si>
-    <t>El estudiante solicita una beca porque su familia tiene un ingreso insuficiente para cubrir las necesidades básicas del hogar y ha excedido la duración nominal de gratuidad.</t>
-  </si>
-  <si>
-    <t>El estudiante solicita una beca debido a su situación económica, encontrándose actualmente cesante y con ingreso informal.</t>
-  </si>
-  <si>
-    <t>El estudiante no tiene deuda vencida que justifique la solicitud de beca.</t>
+    <t>El estudiante solicita una beca porque su situación económica actual es complicada, con ingresos insuficientes en su familia.</t>
+  </si>
+  <si>
+    <t>El estudiante solicita una beca porque excede la duración nominal de gratuidad y tiene un ingreso insuficiente para cubrir las necesidades básicas del hogar.</t>
+  </si>
+  <si>
+    <t>El estudiante solicita una beca por su situación económica que incluye cesantía y un ingreso informal.</t>
+  </si>
+  <si>
+    <t>El estudiante no tiene deuda vencida registrada.</t>
   </si>
   <si>
     <t>El estudiante no tiene deuda vencida en el sistema.</t>
   </si>
   <si>
-    <t>El estudiante solicita una beca para cubrir su deuda vencida y ha sido evaluado positivamente por la Trabajadora Social.</t>
-  </si>
-  <si>
-    <t>El estudiante solicita una beca debido a su situación financiera y se sugiere aprobar la solicitud por su deuda.</t>
-  </si>
-  <si>
-    <t>El estudiante no tiene deuda a cubrir y, por lo tanto, no puede optar a la beca.</t>
-  </si>
-  <si>
-    <t>La Trabajadora Social sugiere rechazar la solicitud debido a la situación económica familiar.</t>
-  </si>
-  <si>
-    <t>El estudiante no tiene deuda a cubrir, por lo que no se aprueba la solicitud de beca.</t>
-  </si>
-  <si>
-    <t>El estudiante solicita una beca 1 arancel y tiene una deuda vencida.</t>
-  </si>
-  <si>
-    <t>El estudiante solicita una beca para cubrir su deuda vencida y tiene una situación socioeconómica vulnerable.</t>
-  </si>
-  <si>
-    <t>El estudiante no cumple con el requisito de deuda pendiente.</t>
-  </si>
-  <si>
-    <t>El estudiante no presenta información suficiente para evaluar su situación.</t>
-  </si>
-  <si>
-    <t>Carta de solicitud de beca; Documentación validada por la Trabajadora Social; Certificado de remuneraciones; FICHA SOCIOECONOMICA</t>
-  </si>
-  <si>
-    <t>Carta de solicitud de beca; FICHA SOCIOECONOMICA; Informe de Trabajadora Social</t>
-  </si>
-  <si>
-    <t>Carta de solicitud de beca; Documentos validados por Trabajadora Social; Informe de situación socioeconómica</t>
-  </si>
-  <si>
-    <t>Documentos validados por la Trabajadora Social; Informe de situación familiar; Postulación al FUAS.</t>
+    <t>El estudiante solicita una beca para cubrir su deuda vencida, y se ha validado su situación por la Trabajadora Social.</t>
+  </si>
+  <si>
+    <t>El estudiante solicita una beca porque tiene una deuda vencida y cumple con los requisitos establecidos.</t>
+  </si>
+  <si>
+    <t>El estudiante solicita una beca porque presenta una situación de deuda y ha sido evaluado positivamente.</t>
+  </si>
+  <si>
+    <t>El estudiante no tiene deuda a cubrir.</t>
+  </si>
+  <si>
+    <t>El estudiante no cumple con el requisito de tener deuda vencida.</t>
+  </si>
+  <si>
+    <t>El estudiante se encuentra en una situación económica desafiante, pero se sugiere rechazar la solicitud por recomendación de la Trabajadora Social.</t>
+  </si>
+  <si>
+    <t>El estudiante tiene deuda vencida de 0.0 en el sistema, lo que impide la aprobación de la beca.</t>
+  </si>
+  <si>
+    <t>El estudiante solicita una beca para ayudar a cubrir la deuda vencida registrada en el sistema.</t>
+  </si>
+  <si>
+    <t>El estudiante solicita una beca 1 arancel debido a su situación económica vulnerable y la validación de documentos por parte de Trabajadora Social.</t>
+  </si>
+  <si>
+    <t>El estudiante no tiene deuda vencida, lo que impide la aprobación de la beca.</t>
+  </si>
+  <si>
+    <t>No se cumple con los requisitos necesarios debido a la falta de datos fundamentales.</t>
   </si>
   <si>
     <t>Carta de solicitud de beca; Cartola Hogar; Certificado de remuneraciones; FICHA SOCIOECONOMICA</t>
   </si>
   <si>
-    <t>Carta de solicitud de beca; Cartola Hogar; Certificado de remuneraciones; FICHA SOCIOECONOMICA; Documentos validados por Trabajadora Social</t>
-  </si>
-  <si>
-    <t>Carta de solicitud de beca; Ficha socioeconómica; Documentos médicos; Validación por Trabajadora Social</t>
-  </si>
-  <si>
-    <t>Carta de solicitud de beca; BECAS Y BENEFICIOS; Documentos validados por la Trabajadora Social</t>
+    <t>Carta de solicitud de beca; Cartola Hogar; Certificado de remuneraciones; Documentación validada por Trabajadora Social</t>
   </si>
   <si>
     <t>Carta de solicitud de beca; FICHA SOCIOECONOMICA</t>
   </si>
   <si>
+    <t>Carta de solicitud de beca; Informe de la Trabajadora Social; Documentación que acredita ingresos; FICHA SOCIOECONOMICA</t>
+  </si>
+  <si>
+    <t>Carta de solicitud de beca; FICHA SOCIOECONOMICA; Certificado médico; Parte policial; Informe de la Trabajadora Social</t>
+  </si>
+  <si>
+    <t>Carta de solicitud de beca; Informe de la Trabajadora Social; Documentos de identidad; Comprobante de ingresos; Certificados de beneficios anteriores</t>
+  </si>
+  <si>
     <t>RSH</t>
-  </si>
-  <si>
-    <t>Carta de solicitud de beca; Documentos validados por Trabajadora Social</t>
   </si>
 </sst>
 </file>
@@ -1316,13 +1316,13 @@
         <v>168</v>
       </c>
       <c r="X2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y2" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z2" t="s">
         <v>187</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -1393,13 +1393,13 @@
         <v>169</v>
       </c>
       <c r="X3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Y3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="Z3" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -1470,13 +1470,13 @@
         <v>170</v>
       </c>
       <c r="X4" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Y4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="Z4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -1547,13 +1547,13 @@
         <v>171</v>
       </c>
       <c r="X5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Y5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="Z5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -1624,13 +1624,13 @@
         <v>172</v>
       </c>
       <c r="X6" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y6" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z6" t="s">
         <v>187</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -1701,13 +1701,13 @@
         <v>172</v>
       </c>
       <c r="X7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y7" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z7" t="s">
         <v>187</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -1778,13 +1778,13 @@
         <v>173</v>
       </c>
       <c r="X8" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y8" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="Z8" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1852,16 +1852,16 @@
         <v>166</v>
       </c>
       <c r="W9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="X9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y9" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="Z9" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -1926,16 +1926,16 @@
         <v>167</v>
       </c>
       <c r="W10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="X10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Y10" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="Z10" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -2000,16 +2000,16 @@
         <v>167</v>
       </c>
       <c r="W11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="X11" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Y11" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="Z11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -2070,6 +2070,21 @@
       <c r="T12">
         <v>281000</v>
       </c>
+      <c r="V12" t="s">
+        <v>167</v>
+      </c>
+      <c r="W12" t="s">
+        <v>177</v>
+      </c>
+      <c r="X12" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="13" spans="1:26">
       <c r="A13" t="s">
@@ -2136,16 +2151,16 @@
         <v>166</v>
       </c>
       <c r="W13" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="X13" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y13" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="Z13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -2213,16 +2228,16 @@
         <v>166</v>
       </c>
       <c r="W14" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="X14" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y14" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="Z14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -2287,16 +2302,16 @@
         <v>166</v>
       </c>
       <c r="W15" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="X15" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y15" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="Z15" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -2361,16 +2376,16 @@
         <v>166</v>
       </c>
       <c r="W16" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="X16" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y16" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z16" t="s">
         <v>187</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -2438,16 +2453,16 @@
         <v>166</v>
       </c>
       <c r="W17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="X17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y17" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="Z17" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:26">
@@ -2515,16 +2530,16 @@
         <v>166</v>
       </c>
       <c r="W18" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="X18" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y18" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="Z18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:26">
@@ -2592,16 +2607,16 @@
         <v>166</v>
       </c>
       <c r="W19" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="X19" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y19" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="Z19" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:26">
@@ -2666,16 +2681,16 @@
         <v>166</v>
       </c>
       <c r="W20" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="X20" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y20" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z20" t="s">
         <v>187</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -2740,13 +2755,13 @@
         <v>167</v>
       </c>
       <c r="W21" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="X21" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Y21" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="Z21" t="s">
         <v>206</v>
@@ -2817,16 +2832,16 @@
         <v>166</v>
       </c>
       <c r="W22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X22" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y22" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z22" t="s">
         <v>187</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:26">
@@ -2894,16 +2909,16 @@
         <v>166</v>
       </c>
       <c r="W23" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="X23" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y23" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z23" t="s">
         <v>187</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:26">
@@ -2971,13 +2986,13 @@
         <v>167</v>
       </c>
       <c r="W24" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="X24" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Y24" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="Z24" t="s">
         <v>206</v>
@@ -3045,16 +3060,16 @@
         <v>166</v>
       </c>
       <c r="W25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="X25" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y25" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="Z25" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:26">
@@ -3122,13 +3137,13 @@
         <v>172</v>
       </c>
       <c r="X26" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y26" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z26" t="s">
         <v>187</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:26">
@@ -3196,16 +3211,16 @@
         <v>166</v>
       </c>
       <c r="W27" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="X27" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y27" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="Z27" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:26">
@@ -3270,16 +3285,16 @@
         <v>166</v>
       </c>
       <c r="W28" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="X28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="Z28" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:26">
@@ -3347,16 +3362,16 @@
         <v>166</v>
       </c>
       <c r="W29" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="X29" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y29" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="Z29" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:26">
@@ -3367,16 +3382,16 @@
         <v>166</v>
       </c>
       <c r="W30" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="X30" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Y30" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="Z30" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>